<commit_message>
comentarios v 27 noviembre 2025
</commit_message>
<xml_diff>
--- a/DATOS/PONDERACIONES/IPC_INQUILINOS/alquiler_ajustado_ponderaciones_IPC_2018.xlsx
+++ b/DATOS/PONDERACIONES/IPC_INQUILINOS/alquiler_ajustado_ponderaciones_IPC_2018.xlsx
@@ -384,7 +384,7 @@
         <v>180.733</v>
       </c>
       <c r="C2">
-        <v>139.8332623247955</v>
+        <v>144.1997889963244</v>
       </c>
     </row>
     <row r="3">
@@ -397,7 +397,7 @@
         <v>13.481</v>
       </c>
       <c r="C3">
-        <v>10.43026015946489</v>
+        <v>10.75596241671111</v>
       </c>
     </row>
     <row r="4">
@@ -410,7 +410,7 @@
         <v>8.497</v>
       </c>
       <c r="C4">
-        <v>6.574135492543072</v>
+        <v>6.779423830190218</v>
       </c>
     </row>
     <row r="5">
@@ -423,7 +423,7 @@
         <v>21.256</v>
       </c>
       <c r="C5">
-        <v>16.44578369183189</v>
+        <v>16.95933069724882</v>
       </c>
     </row>
     <row r="6">
@@ -436,7 +436,7 @@
         <v>49.916</v>
       </c>
       <c r="C6">
-        <v>38.62004792818406</v>
+        <v>39.82602329148816</v>
       </c>
     </row>
     <row r="7">
@@ -449,7 +449,7 @@
         <v>16.66</v>
       </c>
       <c r="C7">
-        <v>12.88985492594652</v>
+        <v>13.29236212910074</v>
       </c>
     </row>
     <row r="8">
@@ -462,7 +462,7 @@
         <v>11.342</v>
       </c>
       <c r="C8">
-        <v>8.775314199885081</v>
+        <v>9.04933801130016</v>
       </c>
     </row>
     <row r="9">
@@ -475,7 +475,7 @@
         <v>36.036</v>
       </c>
       <c r="C9">
-        <v>27.88108115914819</v>
+        <v>28.75171438681119</v>
       </c>
     </row>
     <row r="10">
@@ -488,7 +488,7 @@
         <v>55.82</v>
       </c>
       <c r="C10">
-        <v>43.18797730890365</v>
+        <v>44.53659388033635</v>
       </c>
     </row>
     <row r="11">
@@ -501,7 +501,7 @@
         <v>12.446</v>
       </c>
       <c r="C11">
-        <v>9.6294798564424</v>
+        <v>9.930176414092909</v>
       </c>
     </row>
     <row r="12">
@@ -514,7 +514,7 @@
         <v>5.301</v>
       </c>
       <c r="C12">
-        <v>4.101387812871699</v>
+        <v>4.229460482974972</v>
       </c>
     </row>
     <row r="13">
@@ -527,7 +527,7 @@
         <v>9.336</v>
       </c>
       <c r="C13">
-        <v>7.223270443495601</v>
+        <v>7.448829101877825</v>
       </c>
     </row>
     <row r="14">
@@ -540,7 +540,7 @@
         <v>2.34</v>
       </c>
       <c r="C14">
-        <v>1.810459815529103</v>
+        <v>1.866994440702025</v>
       </c>
     </row>
     <row r="15">
@@ -553,7 +553,7 @@
         <v>2.246</v>
       </c>
       <c r="C15">
-        <v>1.737731942597592</v>
+        <v>1.791995518725106</v>
       </c>
     </row>
     <row r="16">
@@ -566,7 +566,7 @@
         <v>26.789</v>
       </c>
       <c r="C16">
-        <v>20.72667008470476</v>
+        <v>21.37389490254981</v>
       </c>
     </row>
     <row r="17">
@@ -579,7 +579,7 @@
         <v>19.625</v>
       </c>
       <c r="C17">
-        <v>15.18387772639258</v>
+        <v>15.65801961486207</v>
       </c>
     </row>
     <row r="18">
@@ -592,7 +592,7 @@
         <v>18.547</v>
       </c>
       <c r="C18">
-        <v>14.34982829000781</v>
+        <v>14.79792559474379</v>
       </c>
     </row>
     <row r="19">
@@ -605,7 +605,7 @@
         <v>1.366</v>
       </c>
       <c r="C19">
-        <v>1.056875259834511</v>
+        <v>1.08987795128161</v>
       </c>
     </row>
     <row r="20">
@@ -618,7 +618,7 @@
         <v>38.514</v>
       </c>
       <c r="C20">
-        <v>29.79831168174696</v>
+        <v>30.72881362786231</v>
       </c>
     </row>
     <row r="21">
@@ -631,7 +631,7 @@
         <v>90.953</v>
       </c>
       <c r="C21">
-        <v>70.37040666744382</v>
+        <v>72.56783989964586</v>
       </c>
     </row>
     <row r="22">
@@ -644,7 +644,7 @@
         <v>17.975</v>
       </c>
       <c r="C22">
-        <v>13.90727144621181</v>
+        <v>14.34154917590552</v>
       </c>
     </row>
     <row r="23">
@@ -657,7 +657,7 @@
         <v>0.266</v>
       </c>
       <c r="C23">
-        <v>0.2058044063806587</v>
+        <v>0.2122309919772388</v>
       </c>
     </row>
     <row r="24">
@@ -670,7 +670,7 @@
         <v>3.033</v>
       </c>
       <c r="C24">
-        <v>2.346634453205029</v>
+        <v>2.419912025063779</v>
       </c>
     </row>
     <row r="25">
@@ -683,7 +683,7 @@
         <v>33.074</v>
       </c>
       <c r="C25">
-        <v>25.58937946102972</v>
+        <v>26.38845048366615</v>
       </c>
     </row>
     <row r="26">
@@ -696,7 +696,7 @@
         <v>9.75</v>
       </c>
       <c r="C26">
-        <v>7.543582564704596</v>
+        <v>7.779143502925105</v>
       </c>
     </row>
     <row r="27">
@@ -706,10 +706,10 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.72</v>
+        <v>0.7199999999999999</v>
       </c>
       <c r="C27">
-        <v>0.5570645586243393</v>
+        <v>0.5744598279083155</v>
       </c>
     </row>
     <row r="28">
@@ -722,7 +722,7 @@
         <v>13.747</v>
       </c>
       <c r="C28">
-        <v>10.63606456584555</v>
+        <v>10.96819340868835</v>
       </c>
     </row>
     <row r="29">
@@ -735,7 +735,7 @@
         <v>31.537</v>
       </c>
       <c r="C29">
-        <v>24.40020136852193</v>
+        <v>25.16213832325631</v>
       </c>
     </row>
     <row r="30">
@@ -748,7 +748,7 @@
         <v>13.599</v>
       </c>
       <c r="C30">
-        <v>10.52155685101721</v>
+        <v>10.85010999961831</v>
       </c>
     </row>
     <row r="31">
@@ -761,7 +761,7 @@
         <v>16.661</v>
       </c>
       <c r="C31">
-        <v>12.89062862672239</v>
+        <v>13.29315998997284</v>
       </c>
     </row>
     <row r="32">
@@ -774,7 +774,7 @@
         <v>4.66</v>
       </c>
       <c r="C32">
-        <v>3.605445615540864</v>
+        <v>3.718031663962154</v>
       </c>
     </row>
     <row r="33">
@@ -787,7 +787,7 @@
         <v>2.293</v>
       </c>
       <c r="C33">
-        <v>1.774095879063348</v>
+        <v>1.829494979713566</v>
       </c>
     </row>
     <row r="34">
@@ -800,7 +800,7 @@
         <v>6.64</v>
       </c>
       <c r="C34">
-        <v>5.137373151757797</v>
+        <v>5.29779619071002</v>
       </c>
     </row>
     <row r="35">
@@ -813,7 +813,7 @@
         <v>3.067</v>
       </c>
       <c r="C35">
-        <v>2.372940279584513</v>
+        <v>2.447039294715005</v>
       </c>
     </row>
     <row r="36">
@@ -826,7 +826,7 @@
         <v>113.26</v>
       </c>
       <c r="C36">
-        <v>87.62934987471206</v>
+        <v>90.36572237346641</v>
       </c>
     </row>
     <row r="37">
@@ -839,7 +839,7 @@
         <v>10.122</v>
       </c>
       <c r="C37">
-        <v>7.831399253327172</v>
+        <v>8.075947747344403</v>
       </c>
     </row>
     <row r="38">
@@ -852,7 +852,7 @@
         <v>32.795</v>
       </c>
       <c r="C38">
-        <v>25.37351694456279</v>
+        <v>26.16584730035168</v>
       </c>
     </row>
     <row r="39">
@@ -865,7 +865,7 @@
         <v>6.667</v>
       </c>
       <c r="C39">
-        <v>5.158263072706209</v>
+        <v>5.319338434256582</v>
       </c>
     </row>
     <row r="40">
@@ -878,7 +878,7 @@
         <v>4.43</v>
       </c>
       <c r="C40">
-        <v>3.427494437091421</v>
+        <v>3.53452366338033</v>
       </c>
     </row>
     <row r="41">
@@ -891,7 +891,7 @@
         <v>15.411</v>
       </c>
       <c r="C41">
-        <v>11.92350265688846</v>
+        <v>12.29583389985424</v>
       </c>
     </row>
     <row r="42">
@@ -904,7 +904,7 @@
         <v>1.077</v>
       </c>
       <c r="C42">
-        <v>0.8332757356089077</v>
+        <v>0.8592961592461887</v>
       </c>
     </row>
     <row r="43">
@@ -917,7 +917,7 @@
         <v>7.379</v>
       </c>
       <c r="C43">
-        <v>5.709138025123612</v>
+        <v>5.887415375188139</v>
       </c>
     </row>
     <row r="44">
@@ -930,7 +930,7 @@
         <v>30.636</v>
       </c>
       <c r="C44">
-        <v>250</v>
+        <v>226.58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Todos los cambios integrados
</commit_message>
<xml_diff>
--- a/DATOS/PONDERACIONES/IPC_INQUILINOS/alquiler_ajustado_ponderaciones_IPC_2018.xlsx
+++ b/DATOS/PONDERACIONES/IPC_INQUILINOS/alquiler_ajustado_ponderaciones_IPC_2018.xlsx
@@ -384,7 +384,7 @@
         <v>180.733</v>
       </c>
       <c r="C2">
-        <v>144.1997889963244</v>
+        <v>143.1428165540178</v>
       </c>
     </row>
     <row r="3">
@@ -397,7 +397,7 @@
         <v>13.481</v>
       </c>
       <c r="C3">
-        <v>10.75596241671111</v>
+        <v>10.67712210810817</v>
       </c>
     </row>
     <row r="4">
@@ -410,7 +410,7 @@
         <v>8.497</v>
       </c>
       <c r="C4">
-        <v>6.779423830190218</v>
+        <v>6.729731218203035</v>
       </c>
     </row>
     <row r="5">
@@ -423,7 +423,7 @@
         <v>21.256</v>
       </c>
       <c r="C5">
-        <v>16.95933069724882</v>
+        <v>16.83502021585545</v>
       </c>
     </row>
     <row r="6">
@@ -436,7 +436,7 @@
         <v>49.916</v>
       </c>
       <c r="C6">
-        <v>39.82602329148816</v>
+        <v>39.53410185804669</v>
       </c>
     </row>
     <row r="7">
@@ -449,7 +449,7 @@
         <v>16.66</v>
       </c>
       <c r="C7">
-        <v>13.29236212910074</v>
+        <v>13.19493022187391</v>
       </c>
     </row>
     <row r="8">
@@ -462,7 +462,7 @@
         <v>11.342</v>
       </c>
       <c r="C8">
-        <v>9.04933801130016</v>
+        <v>8.983007117436603</v>
       </c>
     </row>
     <row r="9">
@@ -475,7 +475,7 @@
         <v>36.036</v>
       </c>
       <c r="C9">
-        <v>28.75171438681119</v>
+        <v>28.54096671521297</v>
       </c>
     </row>
     <row r="10">
@@ -488,7 +488,7 @@
         <v>55.82</v>
       </c>
       <c r="C10">
-        <v>44.53659388033635</v>
+        <v>44.21014435684282</v>
       </c>
     </row>
     <row r="11">
@@ -501,7 +501,7 @@
         <v>12.446</v>
       </c>
       <c r="C11">
-        <v>9.930176414092909</v>
+        <v>9.8573890481058</v>
       </c>
     </row>
     <row r="12">
@@ -514,7 +514,7 @@
         <v>5.301</v>
       </c>
       <c r="C12">
-        <v>4.229460482974972</v>
+        <v>4.198458889925184</v>
       </c>
     </row>
     <row r="13">
@@ -527,7 +527,7 @@
         <v>9.336</v>
       </c>
       <c r="C13">
-        <v>7.448829101877825</v>
+        <v>7.39422980500689</v>
       </c>
     </row>
     <row r="14">
@@ -540,7 +540,7 @@
         <v>2.34</v>
       </c>
       <c r="C14">
-        <v>1.866994440702025</v>
+        <v>1.853309526961881</v>
       </c>
     </row>
     <row r="15">
@@ -553,7 +553,7 @@
         <v>2.246</v>
       </c>
       <c r="C15">
-        <v>1.791995518725106</v>
+        <v>1.778860340836062</v>
       </c>
     </row>
     <row r="16">
@@ -566,7 +566,7 @@
         <v>26.789</v>
       </c>
       <c r="C16">
-        <v>21.37389490254981</v>
+        <v>21.2172260332401</v>
       </c>
     </row>
     <row r="17">
@@ -579,7 +579,7 @@
         <v>19.625</v>
       </c>
       <c r="C17">
-        <v>15.65801961486207</v>
+        <v>15.54324763531065</v>
       </c>
     </row>
     <row r="18">
@@ -592,7 +592,7 @@
         <v>18.547</v>
       </c>
       <c r="C18">
-        <v>14.79792559474379</v>
+        <v>14.68945803271881</v>
       </c>
     </row>
     <row r="19">
@@ -605,7 +605,7 @@
         <v>1.366</v>
       </c>
       <c r="C19">
-        <v>1.08987795128161</v>
+        <v>1.081889236679457</v>
       </c>
     </row>
     <row r="20">
@@ -618,7 +618,7 @@
         <v>38.514</v>
       </c>
       <c r="C20">
-        <v>30.72881362786231</v>
+        <v>30.5035739835085</v>
       </c>
     </row>
     <row r="21">
@@ -631,7 +631,7 @@
         <v>90.953</v>
       </c>
       <c r="C21">
-        <v>72.56783989964586</v>
+        <v>72.03592367767691</v>
       </c>
     </row>
     <row r="22">
@@ -644,7 +644,7 @@
         <v>17.975</v>
       </c>
       <c r="C22">
-        <v>14.34154917590552</v>
+        <v>14.23642681501701</v>
       </c>
     </row>
     <row r="23">
@@ -657,7 +657,7 @@
         <v>0.266</v>
       </c>
       <c r="C23">
-        <v>0.2122309919772388</v>
+        <v>0.210675356483701</v>
       </c>
     </row>
     <row r="24">
@@ -670,7 +670,7 @@
         <v>3.033</v>
       </c>
       <c r="C24">
-        <v>2.419912025063779</v>
+        <v>2.402174271485207</v>
       </c>
     </row>
     <row r="25">
@@ -683,7 +683,7 @@
         <v>33.074</v>
       </c>
       <c r="C25">
-        <v>26.38845048366615</v>
+        <v>26.1950253396313</v>
       </c>
     </row>
     <row r="26">
@@ -696,7 +696,7 @@
         <v>9.75</v>
       </c>
       <c r="C26">
-        <v>7.779143502925105</v>
+        <v>7.722123029007837</v>
       </c>
     </row>
     <row r="27">
@@ -706,10 +706,10 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.7199999999999999</v>
+        <v>0.72</v>
       </c>
       <c r="C27">
-        <v>0.5744598279083155</v>
+        <v>0.5702490852190403</v>
       </c>
     </row>
     <row r="28">
@@ -722,7 +722,7 @@
         <v>13.747</v>
       </c>
       <c r="C28">
-        <v>10.96819340868835</v>
+        <v>10.88779746459187</v>
       </c>
     </row>
     <row r="29">
@@ -735,7 +735,7 @@
         <v>31.537</v>
       </c>
       <c r="C29">
-        <v>25.16213832325631</v>
+        <v>24.97770194521232</v>
       </c>
     </row>
     <row r="30">
@@ -748,7 +748,7 @@
         <v>13.599</v>
       </c>
       <c r="C30">
-        <v>10.85010999961831</v>
+        <v>10.77057959707462</v>
       </c>
     </row>
     <row r="31">
@@ -761,7 +761,7 @@
         <v>16.661</v>
       </c>
       <c r="C31">
-        <v>13.29315998997284</v>
+        <v>13.19572223449227</v>
       </c>
     </row>
     <row r="32">
@@ -774,7 +774,7 @@
         <v>4.66</v>
       </c>
       <c r="C32">
-        <v>3.718031663962154</v>
+        <v>3.690778801556566</v>
       </c>
     </row>
     <row r="33">
@@ -787,7 +787,7 @@
         <v>2.293</v>
       </c>
       <c r="C33">
-        <v>1.829494979713566</v>
+        <v>1.816084933898972</v>
       </c>
     </row>
     <row r="34">
@@ -800,7 +800,7 @@
         <v>6.64</v>
       </c>
       <c r="C34">
-        <v>5.29779619071002</v>
+        <v>5.258963785908927</v>
       </c>
     </row>
     <row r="35">
@@ -813,7 +813,7 @@
         <v>3.067</v>
       </c>
       <c r="C35">
-        <v>2.447039294715005</v>
+        <v>2.42910270050944</v>
       </c>
     </row>
     <row r="36">
@@ -826,7 +826,7 @@
         <v>113.26</v>
       </c>
       <c r="C36">
-        <v>90.36572237346641</v>
+        <v>89.70334915542848</v>
       </c>
     </row>
     <row r="37">
@@ -839,7 +839,7 @@
         <v>10.122</v>
       </c>
       <c r="C37">
-        <v>8.075947747344403</v>
+        <v>8.016751723037675</v>
       </c>
     </row>
     <row r="38">
@@ -852,7 +852,7 @@
         <v>32.795</v>
       </c>
       <c r="C38">
-        <v>26.16584730035168</v>
+        <v>25.97405381910892</v>
       </c>
     </row>
     <row r="39">
@@ -865,7 +865,7 @@
         <v>6.667</v>
       </c>
       <c r="C39">
-        <v>5.319338434256582</v>
+        <v>5.280348126604641</v>
       </c>
     </row>
     <row r="40">
@@ -878,7 +878,7 @@
         <v>4.43</v>
       </c>
       <c r="C40">
-        <v>3.53452366338033</v>
+        <v>3.508615899333817</v>
       </c>
     </row>
     <row r="41">
@@ -891,7 +891,7 @@
         <v>15.411</v>
       </c>
       <c r="C41">
-        <v>12.29583389985424</v>
+        <v>12.20570646154254</v>
       </c>
     </row>
     <row r="42">
@@ -904,7 +904,7 @@
         <v>1.077</v>
       </c>
       <c r="C42">
-        <v>0.8592961592461887</v>
+        <v>0.8529975899734811</v>
       </c>
     </row>
     <row r="43">
@@ -917,7 +917,7 @@
         <v>7.379</v>
       </c>
       <c r="C43">
-        <v>5.887415375188139</v>
+        <v>5.844261110876803</v>
       </c>
     </row>
     <row r="44">
@@ -930,7 +930,7 @@
         <v>30.636</v>
       </c>
       <c r="C44">
-        <v>226.58</v>
+        <v>232.249104178437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>